<commit_message>
Fix barriers PDF formatting and update link
</commit_message>
<xml_diff>
--- a/assets/docs/barriers.xlsx
+++ b/assets/docs/barriers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9ef3043cba1c89b1/A. Current Projects/Websites/Ecosystem Equity Story Teller Website/Ecosystem Equity Local Website/assets/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{2054CF7D-B8B4-4989-932E-4DF07FDE4507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="14_{2054CF7D-B8B4-4989-932E-4DF07FDE4507}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E4EF12A-AB0C-461C-89DD-0CC59F6ADBBD}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="DCa1euK3pKFdO9IBBsRpjOa4b5+QDJRbVRK1h7xZYiqdK0z0pIJ4LnLqPsedeOMqKnWUj+F/QnouF+UtZ1zcVQ==" workbookSaltValue="vKa6vxVRiewQhs3DPzntAw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="828" activeTab="1" xr2:uid="{93690C6D-34F0-490E-AF09-BCACB62CD009}"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="117">
   <si>
     <t>High cost of implementing sustainable approaches</t>
   </si>
@@ -386,6 +386,13 @@
 The list was developed from a combination of comprehensive literature review and field experience. It was compiled after noticing that many sustainable agriculture projects begin with a solution already in mind, rather than from a clear definition of the problem. Starting from the barrier is intended to shift the focus: understanding the constraint first, then considering which solutions might be relevant. In this way, the barrier definition becomes the entry point for project design, helping to ensure that interventions address real needs rather than applying generic fixes. 
 Barriers reflect the financial, social, institutional, and environmental challenges farmers face. 
 At some point the aim is to turn the fuller database into a project design website linking problems to solutions. If you'd like to participate in that , get in touch.
+Mark Ellis-Jones, Ecosystem Equity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This document lists barriers faced by farmers in adopting sustainable agricultural practices alongside possible solutions. 
+The list was developed from a combination of comprehensive literature review and field experience. It was compiled after noticing that many sustainable agriculture projects begin with a solution already in mind, rather than from a clear definition of the problem. Starting from the barrier is intended to shift the focus: understanding the constraint first, then considering which solutions might be relevant. In this way, the barrier definition becomes the entry point for project design, helping to ensure that interventions address real needs rather than applying generic fixes. 
+Barriers reflect the financial, social, institutional, and environmental challenges farmers face. 
+At some point the aim is to turn the fuller database into a project design website linking problems to solutions. If you'd like to participate in that, get in touch.
 Mark Ellis-Jones, Ecosystem Equity </t>
   </si>
 </sst>
@@ -717,7 +724,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="15">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -895,6 +902,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -940,7 +956,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -963,12 +979,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -990,24 +1000,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1017,10 +1015,40 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1411,7 +1439,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:2" ht="239.65" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="8" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1422,669 +1450,689 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3EEB9D-D4F2-4609-9B28-192038E052CC}">
-  <dimension ref="A1:C59"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B3:D64"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="C57" sqref="C57"/>
+      <selection activeCell="B3" sqref="B3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="9.06640625" style="2"/>
-    <col min="2" max="2" width="40.46484375" style="9" customWidth="1"/>
-    <col min="3" max="3" width="74.9296875" style="3" customWidth="1"/>
-    <col min="4" max="4" width="29.265625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="9.06640625" style="2"/>
+    <col min="2" max="2" width="4.796875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="76.46484375" style="28" customWidth="1"/>
+    <col min="4" max="4" width="95.3984375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="29.265625" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="6" t="s">
+    <row r="3" spans="2:4" ht="171.75" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="B3" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+    </row>
+    <row r="4" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="2:4" s="1" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B5" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="D5" s="7" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="57" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="11">
+    <row r="6" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C6" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="D6" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A3" s="11">
+    <row r="7" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B7" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="C7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A4" s="15">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B8" s="13">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C8" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D8" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A5" s="16"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="14"/>
-    </row>
-    <row r="6" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="11">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B9" s="14"/>
+      <c r="C9" s="24"/>
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="9">
         <v>4</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="C10" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A7" s="11">
+    <row r="11" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B11" s="9">
         <v>5</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C11" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A8" s="11">
+    <row r="12" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B12" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C12" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A9" s="5">
+    <row r="13" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B13" s="5">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C13" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D13" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="5">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="5">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C14" s="22" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D14" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A11" s="5">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B15" s="5">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C15" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D15" s="4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A12" s="5">
+    <row r="16" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B16" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C16" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="D16" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="11">
+    <row r="17" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B17" s="9">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C17" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D17" s="10" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="11">
+    <row r="18" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B18" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A15" s="11">
+    <row r="19" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B19" s="9">
         <v>13</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C19" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="5">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="5">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C20" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="5">
+    <row r="21" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B21" s="5">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D21" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A18" s="11">
+    <row r="22" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B22" s="9">
         <v>16</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C22" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D22" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A19" s="5">
+    <row r="23" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B23" s="5">
         <v>17</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C23" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D23" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A20" s="5">
+    <row r="24" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B24" s="5">
         <v>18</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C24" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" s="5">
+    <row r="25" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B25" s="5">
         <v>19</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C25" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A22" s="5">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B26" s="5">
         <v>20</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C26" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A23" s="5">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B27" s="5">
         <v>21</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C27" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D27" s="4" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A24" s="25">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B28" s="19">
         <v>22</v>
       </c>
-      <c r="B24" s="26" t="s">
+      <c r="C28" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D28" s="4" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A25" s="5">
+    <row r="29" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B29" s="5">
         <v>23</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C29" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D29" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A26" s="5">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B30" s="5">
         <v>24</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C30" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D30" s="4" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A27" s="5">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B31" s="5">
         <v>25</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D31" s="4" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A28" s="5">
+    <row r="32" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B32" s="5">
         <v>26</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C32" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D32" s="4" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A29" s="5">
+    <row r="33" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B33" s="5">
         <v>27</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C33" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D33" s="4" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="5">
+    <row r="34" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B34" s="5">
         <v>28</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C34" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D34" s="4" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A31" s="5">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B35" s="5">
         <v>29</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C35" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C31" s="4" t="s">
+      <c r="D35" s="4" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
+    <row r="36" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B36" s="5">
         <v>30</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="C36" s="21" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="D36" s="4" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A33" s="5">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B37" s="5">
         <v>31</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C37" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="C33" s="4" t="s">
+      <c r="D37" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A34" s="5">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B38" s="5">
         <v>32</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="C38" s="21" t="s">
         <v>57</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="D38" s="4" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A35" s="5">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B39" s="5">
         <v>33</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="C39" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="5">
+    <row r="40" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B40" s="5">
         <v>34</v>
       </c>
-      <c r="B36" s="7" t="s">
+      <c r="C40" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A37" s="5">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B41" s="5">
         <v>35</v>
       </c>
-      <c r="B37" s="7" t="s">
+      <c r="C41" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="D41" s="4" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="5">
+    <row r="42" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B42" s="5">
         <v>36</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="C42" s="21" t="s">
         <v>61</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A39" s="5">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B43" s="5">
         <v>37</v>
       </c>
-      <c r="B39" s="7" t="s">
+      <c r="C43" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="C39" s="4" t="s">
+      <c r="D43" s="4" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A40" s="5">
+    <row r="44" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B44" s="5">
         <v>38</v>
       </c>
-      <c r="B40" s="7" t="s">
+      <c r="C44" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="D44" s="4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A41" s="5">
+    <row r="45" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B45" s="5">
         <v>39</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="C45" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="C41" s="4" t="s">
+      <c r="D45" s="4" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A42" s="5">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B46" s="5">
         <v>40</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C46" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D46" s="4" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A43" s="5">
+    <row r="47" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B47" s="5">
         <v>41</v>
       </c>
-      <c r="B43" s="7" t="s">
+      <c r="C47" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C43" s="4" t="s">
+      <c r="D47" s="4" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A44" s="5">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B48" s="5">
         <v>42</v>
       </c>
-      <c r="B44" s="7" t="s">
+      <c r="C48" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="D48" s="4" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A45" s="5">
+    <row r="49" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B49" s="5">
         <v>43</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="C49" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="D49" s="4" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A46" s="5">
+    <row r="50" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B50" s="5">
         <v>44</v>
       </c>
-      <c r="B46" s="7" t="s">
+      <c r="C50" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="D50" s="4" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A47" s="5">
+    <row r="51" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B51" s="5">
         <v>45</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="C51" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A48" s="5">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B52" s="5">
         <v>46</v>
       </c>
-      <c r="B48" s="7" t="s">
+      <c r="C52" s="21" t="s">
         <v>77</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="D52" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="5">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B53" s="5">
         <v>47</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="C53" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="4" t="s">
+      <c r="D53" s="4" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A50" s="5">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B54" s="5">
         <v>48</v>
       </c>
-      <c r="B50" s="7" t="s">
+      <c r="C54" s="21" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="D54" s="4" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A51" s="25">
+    <row r="55" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B55" s="19">
         <v>49</v>
       </c>
-      <c r="B51" s="26" t="s">
+      <c r="C55" s="25" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="27" t="s">
+      <c r="D55" s="20" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A52" s="5">
+    <row r="56" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B56" s="5">
         <v>50</v>
       </c>
-      <c r="B52" s="7" t="s">
+      <c r="C56" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="D56" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="42.75" x14ac:dyDescent="0.45">
-      <c r="A53" s="5">
+    <row r="57" spans="2:4" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="B57" s="5">
         <v>51</v>
       </c>
-      <c r="B53" s="7" t="s">
+      <c r="C57" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C53" s="4" t="s">
+      <c r="D57" s="4" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="5">
+    <row r="58" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B58" s="5">
         <v>52</v>
       </c>
-      <c r="B54" s="7" t="s">
+      <c r="C58" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="D58" s="4" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A55" s="19">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B59" s="15">
         <v>53</v>
       </c>
-      <c r="B55" s="21" t="s">
+      <c r="C59" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="C55" s="23" t="s">
+      <c r="D59" s="17" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A56" s="20"/>
-      <c r="B56" s="22"/>
-      <c r="C56" s="24"/>
-    </row>
-    <row r="57" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A57" s="5">
+    <row r="60" spans="2:4" x14ac:dyDescent="0.45">
+      <c r="B60" s="16"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="18"/>
+    </row>
+    <row r="61" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B61" s="5">
         <v>54</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C61" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C57" s="4" t="s">
+      <c r="D61" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A58" s="5">
+    <row r="62" spans="2:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B62" s="5">
         <v>55</v>
       </c>
-      <c r="B58" s="7" t="s">
+      <c r="C62" s="21" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="D62" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="59" spans="1:3" s="3" customFormat="1" ht="57" x14ac:dyDescent="0.45">
-      <c r="A59" s="4">
+    <row r="63" spans="2:4" s="3" customFormat="1" ht="57" x14ac:dyDescent="0.45">
+      <c r="B63" s="4">
         <v>56</v>
       </c>
-      <c r="B59" s="7" t="s">
+      <c r="C63" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D63" s="4" t="s">
         <v>100</v>
       </c>
     </row>
+    <row r="64" spans="2:4" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="B64" s="29"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="29"/>
+    </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="70nwVdrECYP4Mk5CgJYOo7Rx2ynKBBZ0GKTjgxhoitW3tvL6DMxIvU0E//rLQHDlVVcVp8D3UlEII/259NO1wA==" saltValue="0ApgW8Brz77y11gKcLeGEA==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
-  <mergeCells count="6">
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A4:A5"/>
+  <mergeCells count="7">
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="B8:B9"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.98425196850393704" right="0.98425196850393704" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>
+  <pageSetup paperSize="9" scale="66" fitToHeight="0" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>